<commit_message>
Going on holiday - doesn't compile. Working on lib.rs in r_descent.
</commit_message>
<xml_diff>
--- a/test_results/DCG.xlsx
+++ b/test_results/DCG.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/al/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/al/repos/metric_space/test_results/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C96CFAA-6B73-7545-9B5F-70F27CC30725}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D450B751-BFB4-5949-9D5F-9C78A90227E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8580" yWindow="1900" windowWidth="46080" windowHeight="22740" activeTab="3" xr2:uid="{55A06231-4334-0E4F-8FA5-A4B0271024B6}"/>
+    <workbookView xWindow="4420" yWindow="1800" windowWidth="46080" windowHeight="22740" activeTab="3" xr2:uid="{55A06231-4334-0E4F-8FA5-A4B0271024B6}"/>
   </bookViews>
   <sheets>
     <sheet name="cube_oct_raw" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
     <sheet name="f32" sheetId="3" r:id="rId3"/>
     <sheet name="compare" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="264" uniqueCount="178">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="265" uniqueCount="179">
   <si>
     <t>Results for Q0....</t>
   </si>
@@ -573,6 +573,9 @@
   </si>
   <si>
     <t>DCG(100) fraction</t>
+  </si>
+  <si>
+    <t>Swarm size = 100</t>
   </si>
 </sst>
 </file>
@@ -2188,10 +2191,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BB6354F9-CDB7-D242-8921-0FB829E7B3F5}">
-  <dimension ref="A1:L23"/>
+  <dimension ref="A1:L24"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="K28" sqref="K28"/>
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2674,6 +2677,11 @@
         <v>174</v>
       </c>
     </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>178</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>